<commit_message>
All core features done
</commit_message>
<xml_diff>
--- a/HabitTrackerDiscordBot.xlsx
+++ b/HabitTrackerDiscordBot.xlsx
@@ -5,83 +5,212 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Acer\Main\Projects_\ProgressTracker\HabitTrackerDiscordBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7635"/>
   </bookViews>
   <sheets>
-    <sheet name="BaseRef" sheetId="2" r:id="rId1"/>
-    <sheet name="Username" sheetId="1" r:id="rId2"/>
+    <sheet name="BaseRef" sheetId="1" r:id="rId1"/>
+    <sheet name="Username" sheetId="2" r:id="rId2"/>
+    <sheet name="lootgoddamn" sheetId="3" r:id="rId3"/>
+    <sheet name="lootgodamn" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+  <si>
+    <t>Base points</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Command name</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>Bonus multiplier</t>
+  </si>
+  <si>
+    <t>Bronze</t>
+  </si>
+  <si>
+    <t>A cool little badge</t>
+  </si>
+  <si>
+    <t>lootgodamn</t>
+  </si>
+  <si>
+    <t>help</t>
+  </si>
+  <si>
+    <t>Shows all commands available for use</t>
+  </si>
+  <si>
+    <t>Duration multi</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>A pretty cool badge</t>
+  </si>
+  <si>
+    <t>lootgoddamn</t>
+  </si>
+  <si>
+    <t>adduser</t>
+  </si>
+  <si>
+    <t>Add a new user to track</t>
+  </si>
+  <si>
+    <t>Difficulty multi</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>A very cool badge</t>
+  </si>
+  <si>
+    <t>Dummy</t>
+  </si>
+  <si>
+    <t>removeuser</t>
+  </si>
+  <si>
+    <t>Remove existing user</t>
+  </si>
+  <si>
+    <t>Importance multi</t>
+  </si>
+  <si>
+    <t>Platinum</t>
+  </si>
+  <si>
+    <t>A super cool badge</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>Add a task for yourself</t>
+  </si>
+  <si>
+    <t>Friction multi</t>
+  </si>
+  <si>
+    <t>Diamond</t>
+  </si>
+  <si>
+    <t>The coolest badge</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>Remove one of your tasks</t>
+  </si>
+  <si>
+    <t>finish</t>
+  </si>
+  <si>
+    <t>Finish one of your tasks</t>
+  </si>
+  <si>
+    <t>Item Amount</t>
+  </si>
+  <si>
+    <t>tasks</t>
+  </si>
+  <si>
+    <t>Show yours or someone else's tasks</t>
+  </si>
+  <si>
+    <t>User Count</t>
+  </si>
+  <si>
+    <t>shop</t>
+  </si>
+  <si>
+    <t>Show items available for purchase</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>Buy an item from the shop</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>stats</t>
+  </si>
+  <si>
+    <t>Show yours or someone else's stats</t>
+  </si>
+  <si>
+    <t>pointsettings</t>
+  </si>
+  <si>
+    <t>Show multipliers for points</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
   <si>
     <t>Task Name</t>
   </si>
   <si>
+    <t>Duration in hours</t>
+  </si>
+  <si>
     <t>Difficulty</t>
   </si>
   <si>
-    <t>Duration in hours</t>
-  </si>
-  <si>
     <t>Importance</t>
   </si>
   <si>
     <t>Friction</t>
   </si>
   <si>
-    <t>Points</t>
-  </si>
-  <si>
-    <t>Base points</t>
-  </si>
-  <si>
-    <t>Bonus multiplier</t>
-  </si>
-  <si>
-    <t>Duration multi</t>
-  </si>
-  <si>
-    <t>Difficulty multi</t>
-  </si>
-  <si>
-    <t>Importance multi</t>
-  </si>
-  <si>
-    <t>Friction multi</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Desc</t>
+    <t>Bought Items</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
   <si>
     <t>Tasks done</t>
   </si>
   <si>
+    <t>Try out commands for the first time</t>
+  </si>
+  <si>
     <t>Daily goal</t>
   </si>
   <si>
     <t>Days maxxed</t>
   </si>
   <si>
-    <t>Users</t>
+    <t>Tasks undone</t>
   </si>
 </sst>
 </file>
@@ -117,11 +246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,92 +532,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
     <col min="4" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>100</v>
       </c>
+      <c r="C1">
+        <v>5</v>
+      </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>2500</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>5000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5">
+        <v>7500</v>
+      </c>
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>50</v>
       </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" t="s">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,58 +788,411 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="5.28515625" customWidth="1"/>
     <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B1">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="J1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>60</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="2.28515625" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>300</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M6">
         <v>0</v>
       </c>
     </row>

</xml_diff>